<commit_message>
Updated the Sprint 4 backlog with progress
1) Updated the Sprint 4 backlog with progress for week 1
</commit_message>
<xml_diff>
--- a/sprints/sprint4/Sprint 4 Backlog Burndown.xlsx
+++ b/sprints/sprint4/Sprint 4 Backlog Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swamp\Desktop\CapstoneGroup3\sprints\sprint3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swamp\Desktop\CapstoneGroup3\sprints\sprint4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA9E161-3DA5-42AD-9589-8F652FE4AC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4457A2FE-9257-4287-88C7-B67EFA444DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17130" yWindow="0" windowWidth="21375" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Related User Story</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Update Ticket Stage</t>
   </si>
   <si>
-    <t>Assign Ticket</t>
-  </si>
-  <si>
     <t>View Ticket Details</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>Update delete User error message</t>
+  </si>
+  <si>
+    <t>Assign Ticket to User</t>
   </si>
 </sst>
 </file>
@@ -413,10 +413,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1470,7 +1470,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1533,7 +1533,9 @@
       <c r="D3" s="7">
         <v>5</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="9">
+        <v>0</v>
+      </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
@@ -1557,7 +1559,7 @@
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>11</v>
@@ -1573,7 +1575,7 @@
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>13</v>
@@ -1589,7 +1591,7 @@
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>13</v>
@@ -1619,9 +1621,15 @@
       <c r="B9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="9"/>
+      <c r="C9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="10">
+        <v>4</v>
+      </c>
+      <c r="E9" s="9">
+        <v>4</v>
+      </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -1631,7 +1639,9 @@
       <c r="B10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="D10" s="10"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -1641,11 +1651,17 @@
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="10">
+        <v>4</v>
+      </c>
+      <c r="E11" s="9">
+        <v>4</v>
+      </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
@@ -1653,7 +1669,7 @@
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -1962,11 +1978,11 @@
       <c r="C42" s="1"/>
       <c r="D42" s="1">
         <f>SUM(D3:D41)</f>
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E42" s="1">
         <f t="shared" ref="E42:H42" si="0">SUM(E3:E41)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" si="0"/>
@@ -2002,6 +2018,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B208BF211488B4F880DF934C5C83A74" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ea6ebcb2e074b139db49da06cf4ed1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71b55cd54d0ee2f4121790f6a497c1d7" ns2:_="">
     <xsd:import namespace="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d"/>
@@ -2145,15 +2170,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
   <ds:schemaRefs>
@@ -2164,6 +2180,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D5C3914-7DAF-4B4D-BA97-A88E18DCB9DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2179,12 +2203,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added ellipses to ticket
1) Added ellipses control to displayed tickets
</commit_message>
<xml_diff>
--- a/sprints/sprint4/Sprint 4 Backlog Burndown.xlsx
+++ b/sprints/sprint4/Sprint 4 Backlog Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swamp\Desktop\CapstoneGroup3\sprints\sprint4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4457A2FE-9257-4287-88C7-B67EFA444DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C7F767-3CF5-4E23-A543-325C0F177D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1470,7 +1470,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1630,7 +1630,9 @@
       <c r="E9" s="9">
         <v>4</v>
       </c>
-      <c r="F9" s="9"/>
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
@@ -1662,7 +1664,9 @@
       <c r="E11" s="9">
         <v>4</v>
       </c>
-      <c r="F11" s="9"/>
+      <c r="F11" s="9">
+        <v>0</v>
+      </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
     </row>
@@ -2012,18 +2016,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2171,18 +2175,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Revert "Feature create ticket"
</commit_message>
<xml_diff>
--- a/sprints/sprint4/Sprint 4 Backlog Burndown.xlsx
+++ b/sprints/sprint4/Sprint 4 Backlog Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swamp\Desktop\CapstoneGroup3\sprints\sprint4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C7F767-3CF5-4E23-A543-325C0F177D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4457A2FE-9257-4287-88C7-B67EFA444DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1470,7 +1470,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1630,9 +1630,7 @@
       <c r="E9" s="9">
         <v>4</v>
       </c>
-      <c r="F9" s="9">
-        <v>0</v>
-      </c>
+      <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
@@ -1664,9 +1662,7 @@
       <c r="E11" s="9">
         <v>4</v>
       </c>
-      <c r="F11" s="9">
-        <v>0</v>
-      </c>
+      <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
     </row>
@@ -2016,18 +2012,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2175,18 +2171,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated Sprint 4 Backlog Burndown
</commit_message>
<xml_diff>
--- a/sprints/sprint4/Sprint 4 Backlog Burndown.xlsx
+++ b/sprints/sprint4/Sprint 4 Backlog Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swamp\Desktop\CapstoneGroup3\sprints\sprint4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eo00037\source\repos\CapstoneGroup3\sprints\sprint4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C7F767-3CF5-4E23-A543-325C0F177D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0298AE3-4163-42CE-854F-BE2EBDEDA98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Related User Story</t>
   </si>
@@ -413,10 +413,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1470,7 +1470,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1551,7 +1551,9 @@
       <c r="D4" s="7">
         <v>3</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="9">
+        <v>4</v>
+      </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1567,7 +1569,9 @@
       <c r="D5" s="7">
         <v>1</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="9">
+        <v>4</v>
+      </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
@@ -1675,9 +1679,15 @@
       <c r="B12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="9"/>
+      <c r="C12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="10">
+        <v>4</v>
+      </c>
+      <c r="E12" s="9">
+        <v>6</v>
+      </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -1982,11 +1992,11 @@
       <c r="C42" s="1"/>
       <c r="D42" s="1">
         <f>SUM(D3:D41)</f>
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E42" s="1">
         <f t="shared" ref="E42:H42" si="0">SUM(E3:E41)</f>
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" si="0"/>
@@ -2016,18 +2026,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2175,18 +2185,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update Sprint 4 Backlog Burndown.xlsx
</commit_message>
<xml_diff>
--- a/sprints/sprint4/Sprint 4 Backlog Burndown.xlsx
+++ b/sprints/sprint4/Sprint 4 Backlog Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eo00037\source\repos\CapstoneGroup3\sprints\sprint4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0298AE3-4163-42CE-854F-BE2EBDEDA98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB421801-E2DD-4870-BF24-037992DDA8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -416,10 +416,10 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1470,7 +1470,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1570,9 +1570,11 @@
         <v>1</v>
       </c>
       <c r="E5" s="9">
+        <v>2</v>
+      </c>
+      <c r="F5" s="9">
         <v>4</v>
       </c>
-      <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
     </row>
@@ -1685,10 +1687,10 @@
       <c r="D12" s="10">
         <v>4</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9">
         <v>6</v>
       </c>
-      <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
     </row>
@@ -1996,11 +1998,11 @@
       </c>
       <c r="E42" s="1">
         <f t="shared" ref="E42:H42" si="0">SUM(E3:E41)</f>
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G42" s="1">
         <f t="shared" si="0"/>
@@ -2026,18 +2028,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2185,18 +2187,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated sprint 4 backlog with my estimated and actual worked hours
</commit_message>
<xml_diff>
--- a/sprints/sprint4/Sprint 4 Backlog Burndown.xlsx
+++ b/sprints/sprint4/Sprint 4 Backlog Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eo00037\source\repos\CapstoneGroup3\sprints\sprint4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ja00069\Downloads\CapstoneGroup3\sprints\sprint4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB421801-E2DD-4870-BF24-037992DDA8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69358FC-D37F-4C04-B2B1-C90FB73A02C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="10368" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -413,13 +413,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1470,19 +1470,19 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="2" width="54.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="2" width="54.88671875" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="7.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -1502,7 +1502,7 @@
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -1520,7 +1520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
@@ -1540,7 +1540,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
         <v>16</v>
@@ -1558,7 +1558,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
         <v>21</v>
@@ -1578,7 +1578,7 @@
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="7" t="s">
         <v>23</v>
@@ -1589,12 +1589,16 @@
       <c r="D6" s="7">
         <v>3</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="E6" s="9">
+        <v>2</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7" t="s">
         <v>22</v>
@@ -1605,12 +1609,16 @@
       <c r="D7" s="7">
         <v>3</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+      <c r="E7" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1620,7 +1628,7 @@
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>17</v>
       </c>
@@ -1642,7 +1650,7 @@
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="10" t="s">
         <v>19</v>
@@ -1650,13 +1658,19 @@
       <c r="C10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="D10" s="10">
+        <v>6</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9">
+        <v>7</v>
+      </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="10" t="s">
         <v>24</v>
@@ -1676,7 +1690,7 @@
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="10" t="s">
         <v>20</v>
@@ -1694,7 +1708,7 @@
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -1704,7 +1718,7 @@
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -1714,7 +1728,7 @@
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -1724,7 +1738,7 @@
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -1734,7 +1748,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -1744,7 +1758,7 @@
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -1754,7 +1768,7 @@
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -1764,7 +1778,7 @@
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -1774,7 +1788,7 @@
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -1784,7 +1798,7 @@
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
     </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -1794,7 +1808,7 @@
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="13"/>
       <c r="C23" s="5"/>
@@ -1804,7 +1818,7 @@
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
     </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="13"/>
       <c r="C24" s="5"/>
@@ -1814,7 +1828,7 @@
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
     </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1824,7 +1838,7 @@
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -1834,7 +1848,7 @@
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15"/>
       <c r="B27" s="16"/>
       <c r="C27" s="15"/>
@@ -1844,7 +1858,7 @@
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15"/>
       <c r="B28" s="16"/>
       <c r="C28" s="15"/>
@@ -1854,7 +1868,7 @@
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15"/>
       <c r="B29" s="16"/>
       <c r="C29" s="15"/>
@@ -1864,7 +1878,7 @@
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="17"/>
       <c r="B30" s="17"/>
       <c r="C30" s="18"/>
@@ -1874,7 +1888,7 @@
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="17"/>
       <c r="B31" s="17"/>
       <c r="C31" s="18"/>
@@ -1884,7 +1898,7 @@
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -1894,7 +1908,7 @@
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="17"/>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
@@ -1904,7 +1918,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="20"/>
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
@@ -1914,7 +1928,7 @@
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
@@ -1924,7 +1938,7 @@
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -1934,7 +1948,7 @@
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>
@@ -1944,7 +1958,7 @@
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="20"/>
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
@@ -1954,7 +1968,7 @@
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="20"/>
       <c r="B39" s="20"/>
       <c r="C39" s="20"/>
@@ -1964,7 +1978,7 @@
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -1974,7 +1988,7 @@
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
       <c r="B41" s="19" t="s">
         <v>9</v>
@@ -1986,7 +2000,7 @@
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="2" t="s">
         <v>10</v>
@@ -1994,15 +2008,15 @@
       <c r="C42" s="1"/>
       <c r="D42" s="1">
         <f>SUM(D3:D41)</f>
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E42" s="1">
         <f t="shared" ref="E42:H42" si="0">SUM(E3:E41)</f>
-        <v>14</v>
+        <v>16.5</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G42" s="1">
         <f t="shared" si="0"/>
@@ -2028,18 +2042,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2187,18 +2201,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>